<commit_message>
ran the usual files
</commit_message>
<xml_diff>
--- a/data/538Data/rawData/standings/standings.xlsx
+++ b/data/538Data/rawData/standings/standings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="2160" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="2160" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="15" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="week13" sheetId="12" r:id="rId13"/>
     <sheet name="week14" sheetId="13" r:id="rId14"/>
     <sheet name="week15" sheetId="16" r:id="rId15"/>
+    <sheet name="week16" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="494">
   <si>
     <t>Philadelphia1-0</t>
   </si>
@@ -1424,6 +1425,102 @@
   </si>
   <si>
     <t>Oakland3-10</t>
+  </si>
+  <si>
+    <t>New Orleans12-2</t>
+  </si>
+  <si>
+    <t>Kansas City11-3</t>
+  </si>
+  <si>
+    <t>L.A. Chargers11-3</t>
+  </si>
+  <si>
+    <t>New England9-5</t>
+  </si>
+  <si>
+    <t>L.A. Rams11-3</t>
+  </si>
+  <si>
+    <t>Pittsburgh8-5-1</t>
+  </si>
+  <si>
+    <t>Chicago10-4</t>
+  </si>
+  <si>
+    <t>Philadelphia7-7</t>
+  </si>
+  <si>
+    <t>Baltimore8-6</t>
+  </si>
+  <si>
+    <t>Seattle8-6</t>
+  </si>
+  <si>
+    <t>Minnesota7-6-1</t>
+  </si>
+  <si>
+    <t>Dallas8-6</t>
+  </si>
+  <si>
+    <t>Tennessee8-6</t>
+  </si>
+  <si>
+    <t>Houston10-4</t>
+  </si>
+  <si>
+    <t>Indianapolis8-6</t>
+  </si>
+  <si>
+    <t>Carolina6-8</t>
+  </si>
+  <si>
+    <t>Atlanta5-9</t>
+  </si>
+  <si>
+    <t>Denver6-8</t>
+  </si>
+  <si>
+    <t>Detroit5-9</t>
+  </si>
+  <si>
+    <t>Green Bay5-8-1</t>
+  </si>
+  <si>
+    <t>Washington7-7</t>
+  </si>
+  <si>
+    <t>Tampa Bay5-9</t>
+  </si>
+  <si>
+    <t>Miami7-7</t>
+  </si>
+  <si>
+    <t>N.Y. Giants5-9</t>
+  </si>
+  <si>
+    <t>Cleveland6-7-1</t>
+  </si>
+  <si>
+    <t>Jacksonville4-10</t>
+  </si>
+  <si>
+    <t>Cincinnati6-8</t>
+  </si>
+  <si>
+    <t>Buffalo5-9</t>
+  </si>
+  <si>
+    <t>San Francisco4-10</t>
+  </si>
+  <si>
+    <t>N.Y. Jets4-10</t>
+  </si>
+  <si>
+    <t>Arizona3-11</t>
+  </si>
+  <si>
+    <t>Oakland3-11</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="75">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1756,6 +1853,162 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEDCF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FABDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF40ABE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0E3F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAF6FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0190D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF71C0E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF229EDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F4FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF41ABE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4CB0E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEFF9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9CD3EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3FAFD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF97D1EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3DEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0993D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6CBFE7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0C94D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1096D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF89CBEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF6FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF219EDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95D0EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3F3FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1770,7 +2023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1937,6 +2190,87 @@
     <xf numFmtId="9" fontId="3" fillId="48" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="49" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="53" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="57" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="59" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="60" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="61" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="62" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="63" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="64" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="65" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="66" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="67" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="68" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="70" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="71" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="72" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="73" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="74" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14288,6 +14622,1771 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="609600" y="10477500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="NO-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="KC-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="LAC-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1143000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="NE-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1714500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="LAR-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2286000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="PIT-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2857500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="CHI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3238500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="PHI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3619500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="BAL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="4000500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="SEA-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="4381500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="MIN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="4762500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="DAL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5143500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="TEN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="HOU-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="IND-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6096000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="CAR-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6477000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="ATL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6858000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="DEN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7239000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="DET-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7620000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="GB-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8001000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="WSH-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8382000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22" descr="TB-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8763000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23" descr="MIA-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="9144000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24" descr="NYG-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="9525000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="CLE-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10096500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="JAX-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10477500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="CIN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10858500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="BUF-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="SF-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="11620500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="NYJ-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="12192000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="ARI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="12573000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="OAK-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="12954000"/>
           <a:ext cx="266700" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -34952,8 +37051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35694,6 +37793,780 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId33"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1724</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" s="25">
+        <v>0.99</v>
+      </c>
+      <c r="G2" s="56">
+        <v>0.32</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1672</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E3" s="57">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="58">
+        <v>0.75</v>
+      </c>
+      <c r="G3" s="38">
+        <v>0.17</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1641</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="60">
+        <v>0.08</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1626</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" s="62">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>1614</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F6" s="63">
+        <v>0.87</v>
+      </c>
+      <c r="G6" s="64">
+        <v>0.09</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1608</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D7" s="65">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="66">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="41">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.04</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>1598</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F8" s="67">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1596</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="D9" s="68">
+        <v>0.39</v>
+      </c>
+      <c r="E9" s="69">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1588</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="D10" s="70">
+        <v>0.41</v>
+      </c>
+      <c r="E10" s="71">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="37">
+        <v>0.02</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>1580</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="D11" s="72">
+        <v>0.96</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G11" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1560</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="D12" s="73">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1557</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="D13" s="74">
+        <v>0.95</v>
+      </c>
+      <c r="E13" s="75">
+        <v>0.94</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1551</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="D14" s="76">
+        <v>0.46</v>
+      </c>
+      <c r="E14" s="77">
+        <v>0.08</v>
+      </c>
+      <c r="F14" s="41">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="41">
+        <v>0.01</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1542</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15" s="78">
+        <v>0.87</v>
+      </c>
+      <c r="F15" s="79">
+        <v>0.42</v>
+      </c>
+      <c r="G15" s="52">
+        <v>0.04</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1538</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D16" s="80">
+        <v>0.34</v>
+      </c>
+      <c r="E16" s="50">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>1500</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1483</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1473</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1462</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>1461</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1442</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="D22" s="82">
+        <v>0.11</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>1434</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>1426</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D24" s="50">
+        <v>0.05</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>1420</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1418</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>1416</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>1412</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>1401</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>1400</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>1348</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>1339</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>1329</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" location="no" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - no"/>
+    <hyperlink ref="C3" r:id="rId2" location="kc" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - kc"/>
+    <hyperlink ref="C4" r:id="rId3" location="lac" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - lac"/>
+    <hyperlink ref="C5" r:id="rId4" location="ne" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ne"/>
+    <hyperlink ref="C6" r:id="rId5" location="lar" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - lar"/>
+    <hyperlink ref="C7" r:id="rId6" location="pit" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - pit"/>
+    <hyperlink ref="C8" r:id="rId7" location="chi" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - chi"/>
+    <hyperlink ref="C9" r:id="rId8" location="phi" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - phi"/>
+    <hyperlink ref="C10" r:id="rId9" location="bal" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - bal"/>
+    <hyperlink ref="C11" r:id="rId10" location="sea" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - sea"/>
+    <hyperlink ref="C12" r:id="rId11" location="min" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - min"/>
+    <hyperlink ref="C13" r:id="rId12" location="dal" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - dal"/>
+    <hyperlink ref="C14" r:id="rId13" location="ten" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ten"/>
+    <hyperlink ref="C15" r:id="rId14" location="hou" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - hou"/>
+    <hyperlink ref="C16" r:id="rId15" location="ind" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ind"/>
+    <hyperlink ref="C17" r:id="rId16" location="car" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - car"/>
+    <hyperlink ref="C18" r:id="rId17" location="atl" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - atl"/>
+    <hyperlink ref="C19" r:id="rId18" location="den" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - den"/>
+    <hyperlink ref="C20" r:id="rId19" location="det" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - det"/>
+    <hyperlink ref="C21" r:id="rId20" location="gb" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - gb"/>
+    <hyperlink ref="C22" r:id="rId21" location="wsh" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - wsh"/>
+    <hyperlink ref="C23" r:id="rId22" location="tb" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - tb"/>
+    <hyperlink ref="C24" r:id="rId23" location="mia" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - mia"/>
+    <hyperlink ref="C25" r:id="rId24" location="nyg" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - nyg"/>
+    <hyperlink ref="C26" r:id="rId25" location="cle" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - cle"/>
+    <hyperlink ref="C27" r:id="rId26" location="jax" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - jax"/>
+    <hyperlink ref="C28" r:id="rId27" location="cin" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - cin"/>
+    <hyperlink ref="C29" r:id="rId28" location="buf" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - buf"/>
+    <hyperlink ref="C30" r:id="rId29" location="sf" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - sf"/>
+    <hyperlink ref="C31" r:id="rId30" location="nyj" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - nyj"/>
+    <hyperlink ref="C32" r:id="rId31" location="ari" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ari"/>
+    <hyperlink ref="C33" r:id="rId32" location="oak" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - oak"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
+  <drawing r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ran daily files and final 538 data
</commit_message>
<xml_diff>
--- a/data/538Data/rawData/standings/standings.xlsx
+++ b/data/538Data/rawData/standings/standings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="2160" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="2160" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="15" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="week14" sheetId="13" r:id="rId14"/>
     <sheet name="week15" sheetId="16" r:id="rId15"/>
     <sheet name="week16" sheetId="17" r:id="rId16"/>
+    <sheet name="week17" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="526">
   <si>
     <t>Philadelphia1-0</t>
   </si>
@@ -1521,6 +1522,102 @@
   </si>
   <si>
     <t>Oakland3-11</t>
+  </si>
+  <si>
+    <t>New Orleans13-2</t>
+  </si>
+  <si>
+    <t>Kansas City11-4</t>
+  </si>
+  <si>
+    <t>New England10-5</t>
+  </si>
+  <si>
+    <t>L.A. Rams12-3</t>
+  </si>
+  <si>
+    <t>Baltimore9-6</t>
+  </si>
+  <si>
+    <t>Chicago11-4</t>
+  </si>
+  <si>
+    <t>L.A. Chargers11-4</t>
+  </si>
+  <si>
+    <t>Philadelphia8-7</t>
+  </si>
+  <si>
+    <t>Seattle9-6</t>
+  </si>
+  <si>
+    <t>Pittsburgh8-6-1</t>
+  </si>
+  <si>
+    <t>Minnesota8-6-1</t>
+  </si>
+  <si>
+    <t>Dallas9-6</t>
+  </si>
+  <si>
+    <t>Tennessee9-6</t>
+  </si>
+  <si>
+    <t>Indianapolis9-6</t>
+  </si>
+  <si>
+    <t>Houston10-5</t>
+  </si>
+  <si>
+    <t>Atlanta6-9</t>
+  </si>
+  <si>
+    <t>Green Bay6-8-1</t>
+  </si>
+  <si>
+    <t>Carolina6-9</t>
+  </si>
+  <si>
+    <t>Jacksonville5-10</t>
+  </si>
+  <si>
+    <t>Denver6-9</t>
+  </si>
+  <si>
+    <t>Detroit5-10</t>
+  </si>
+  <si>
+    <t>Cleveland7-7-1</t>
+  </si>
+  <si>
+    <t>Washington7-8</t>
+  </si>
+  <si>
+    <t>Tampa Bay5-10</t>
+  </si>
+  <si>
+    <t>N.Y. Giants5-10</t>
+  </si>
+  <si>
+    <t>Miami7-8</t>
+  </si>
+  <si>
+    <t>Cincinnati6-9</t>
+  </si>
+  <si>
+    <t>Buffalo5-10</t>
+  </si>
+  <si>
+    <t>San Francisco4-11</t>
+  </si>
+  <si>
+    <t>Oakland4-11</t>
+  </si>
+  <si>
+    <t>N.Y. Jets4-11</t>
+  </si>
+  <si>
+    <t>Arizona3-12</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1661,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="75">
+  <fills count="91">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2009,6 +2106,102 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADDBF1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1397D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1A9AD9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5EDF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1B9BD9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1196D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF28A1DC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEF8FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF7FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7E0F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7EDF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF48AEE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF61B9E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1EBF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FD5EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF49AFE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2023,7 +2216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2271,6 +2464,54 @@
     <xf numFmtId="9" fontId="3" fillId="74" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="75" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="76" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="77" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="78" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="79" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="80" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="81" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="82" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="83" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="84" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="85" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="86" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="87" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="88" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="89" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="90" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16387,6 +16628,1771 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="609600" y="12954000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="NO-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="KC-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="NE-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1228725"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="LAR-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1885950"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="BAL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2543175"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="CHI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3009900"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="LAC-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="3476625"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="PHI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="4133850"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="SEA-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="4600575"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="PIT-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5067300"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="MIN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="5534025"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="DAL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6000750"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="TEN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6276975"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="IND-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6743700"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="HOU-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7210425"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="ATL-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7677150"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="GB-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8143875"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="CAR-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8610600"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="JAX-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="9077325"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="DEN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="9544050"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="DET-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10010775"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22" descr="CLE-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10477500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23" descr="WSH-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="10944225"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24" descr="TB-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="11410950"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>523875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="NYG-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="11877675"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="MIA-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="12534900"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="CIN-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="13001625"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="BUF-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="13468350"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="SF-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="13935075"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="OAK-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="14592300"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="NYJ-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="15059025"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="ARI-logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="15525750"/>
           <a:ext cx="266700" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -37800,8 +39806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38567,6 +40573,779 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>
   <drawing r:id="rId34"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1730</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="G2" s="83">
+        <v>0.32</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1649</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E3" s="84">
+        <v>0.93</v>
+      </c>
+      <c r="F3" s="85">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="86">
+        <v>0.16</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1634</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F4" s="87">
+        <v>0.89</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.12</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1627</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F5" s="88">
+        <v>0.93</v>
+      </c>
+      <c r="G5" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>1624</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="D6" s="89">
+        <v>0.84</v>
+      </c>
+      <c r="E6" s="89">
+        <v>0.84</v>
+      </c>
+      <c r="F6" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1609</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F7" s="90">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G7" s="50">
+        <v>0.05</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>1605</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E8" s="91">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F8" s="91">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G8" s="30">
+        <v>0.04</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1603</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="D9" s="92">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1603</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G10" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>1602</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="D11" s="93">
+        <v>0.16</v>
+      </c>
+      <c r="E11" s="93">
+        <v>0.16</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1586</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D12" s="94">
+        <v>0.72</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" s="37">
+        <v>0.02</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1567</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1563</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="D14" s="95">
+        <v>0.62</v>
+      </c>
+      <c r="E14" s="96">
+        <v>0.18</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="54">
+        <v>0.02</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1541</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="D15" s="97">
+        <v>0.38</v>
+      </c>
+      <c r="E15" s="82">
+        <v>0.11</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1535</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E16" s="98">
+        <v>0.71</v>
+      </c>
+      <c r="F16" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>1518</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1477</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1465</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1446</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>1440</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1436</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>1435</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>1431</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>1425</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1417</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>1396</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>1395</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>1394</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>1389</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>1363</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>1332</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>1326</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" location="no" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - no"/>
+    <hyperlink ref="C3" r:id="rId2" location="kc" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - kc"/>
+    <hyperlink ref="C4" r:id="rId3" location="ne" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ne"/>
+    <hyperlink ref="C5" r:id="rId4" location="lar" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - lar"/>
+    <hyperlink ref="C6" r:id="rId5" location="bal" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - bal"/>
+    <hyperlink ref="C7" r:id="rId6" location="chi" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - chi"/>
+    <hyperlink ref="C8" r:id="rId7" location="lac" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - lac"/>
+    <hyperlink ref="C9" r:id="rId8" location="phi" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - phi"/>
+    <hyperlink ref="C10" r:id="rId9" location="sea" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - sea"/>
+    <hyperlink ref="C11" r:id="rId10" location="pit" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - pit"/>
+    <hyperlink ref="C12" r:id="rId11" location="min" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - min"/>
+    <hyperlink ref="C13" r:id="rId12" location="dal" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - dal"/>
+    <hyperlink ref="C14" r:id="rId13" location="ten" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ten"/>
+    <hyperlink ref="C15" r:id="rId14" location="ind" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ind"/>
+    <hyperlink ref="C16" r:id="rId15" location="hou" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - hou"/>
+    <hyperlink ref="C17" r:id="rId16" location="atl" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - atl"/>
+    <hyperlink ref="C18" r:id="rId17" location="gb" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - gb"/>
+    <hyperlink ref="C19" r:id="rId18" location="car" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - car"/>
+    <hyperlink ref="C20" r:id="rId19" location="jax" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - jax"/>
+    <hyperlink ref="C21" r:id="rId20" location="den" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - den"/>
+    <hyperlink ref="C22" r:id="rId21" location="det" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - det"/>
+    <hyperlink ref="C23" r:id="rId22" location="cle" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - cle"/>
+    <hyperlink ref="C24" r:id="rId23" location="wsh" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - wsh"/>
+    <hyperlink ref="C25" r:id="rId24" location="tb" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - tb"/>
+    <hyperlink ref="C26" r:id="rId25" location="nyg" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - nyg"/>
+    <hyperlink ref="C27" r:id="rId26" location="mia" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - mia"/>
+    <hyperlink ref="C28" r:id="rId27" location="cin" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - cin"/>
+    <hyperlink ref="C29" r:id="rId28" location="buf" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - buf"/>
+    <hyperlink ref="C30" r:id="rId29" location="sf" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - sf"/>
+    <hyperlink ref="C31" r:id="rId30" location="oak" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - oak"/>
+    <hyperlink ref="C32" r:id="rId31" location="nyj" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - nyj"/>
+    <hyperlink ref="C33" r:id="rId32" location="ari" display="https://projects.fivethirtyeight.com/complete-history-of-the-nfl/ - ari"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>